<commit_message>
upgrade left table until javakheti
</commit_message>
<xml_diff>
--- a/municipal/ENG/Demography/Number of deaths by age and sex/Kareli.xlsx
+++ b/municipal/ENG/Demography/Number of deaths by age and sex/Kareli.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\დემოგრაფია\Tamunas cxrilebi\inglisuri\cx 11 - eng\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gamashukeli\Desktop\demo\demo\2) გარდაცვალება 2022\4(+გარდაცვალება ასაკის და სქესი\Number of deaths by age and sex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FABB079D-1AE5-455D-A177-15DFA8E323DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC340910-3E53-4A9B-8DA2-8645E1323FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3120" windowWidth="28800" windowHeight="8820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterate="1" iterateCount="1000" calcOnSave="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
   <si>
     <t>1-4</t>
   </si>
@@ -106,7 +106,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +150,17 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -353,7 +364,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -429,6 +440,33 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -711,17 +749,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y25"/>
+  <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="20.5703125" style="24" customWidth="1"/>
     <col min="2" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" s="16" customFormat="1" ht="15">
       <c r="A1" s="14" t="s">
         <v>24</v>
       </c>
@@ -750,7 +790,7 @@
       <c r="X1" s="15"/>
       <c r="Y1" s="15"/>
     </row>
-    <row r="2" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" s="16" customFormat="1">
       <c r="A2" s="17"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -777,7 +817,7 @@
       <c r="X2" s="15"/>
       <c r="Y2" s="15"/>
     </row>
-    <row r="3" spans="1:25" s="16" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" s="16" customFormat="1" ht="13.5" thickBot="1">
       <c r="A3" s="18" t="s">
         <v>18</v>
       </c>
@@ -806,7 +846,7 @@
       <c r="X3" s="15"/>
       <c r="Y3" s="15"/>
     </row>
-    <row r="4" spans="1:25" s="16" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" s="16" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A4" s="28" t="s">
         <v>19</v>
       </c>
@@ -850,8 +890,18 @@
       </c>
       <c r="X4" s="26"/>
       <c r="Y4" s="27"/>
+      <c r="Z4" s="25">
+        <v>2022</v>
+      </c>
+      <c r="AA4" s="26"/>
+      <c r="AB4" s="27"/>
+      <c r="AC4" s="25">
+        <v>2023</v>
+      </c>
+      <c r="AD4" s="26"/>
+      <c r="AE4" s="27"/>
     </row>
-    <row r="5" spans="1:25" s="16" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" s="16" customFormat="1" ht="26.25" thickBot="1">
       <c r="A5" s="29"/>
       <c r="B5" s="19" t="s">
         <v>20</v>
@@ -925,8 +975,26 @@
       <c r="Y5" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="Z5" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA5" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB5" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC5" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD5" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE5" s="21" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="6" spans="1:25" s="23" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" s="23" customFormat="1" ht="16.5" customHeight="1">
       <c r="A6" s="22" t="s">
         <v>23</v>
       </c>
@@ -1002,8 +1070,26 @@
       <c r="Y6" s="3">
         <v>283</v>
       </c>
+      <c r="Z6" s="1">
+        <v>499</v>
+      </c>
+      <c r="AA6" s="2">
+        <v>280</v>
+      </c>
+      <c r="AB6" s="3">
+        <v>219</v>
+      </c>
+      <c r="AC6" s="30">
+        <v>453</v>
+      </c>
+      <c r="AD6" s="31">
+        <v>250</v>
+      </c>
+      <c r="AE6" s="32">
+        <v>203</v>
+      </c>
     </row>
-    <row r="7" spans="1:25" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" s="16" customFormat="1" ht="16.5" customHeight="1">
       <c r="A7" s="4">
         <v>0</v>
       </c>
@@ -1079,8 +1165,26 @@
       <c r="Y7" s="7">
         <v>2</v>
       </c>
+      <c r="Z7" s="5">
+        <v>4</v>
+      </c>
+      <c r="AA7" s="6">
+        <v>3</v>
+      </c>
+      <c r="AB7" s="7">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="33">
+        <v>2</v>
+      </c>
+      <c r="AD7" s="34">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="35">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:25" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" s="16" customFormat="1" ht="16.5" customHeight="1">
       <c r="A8" s="8" t="s">
         <v>0</v>
       </c>
@@ -1156,8 +1260,26 @@
       <c r="Y8" s="7">
         <v>1</v>
       </c>
+      <c r="Z8" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="7">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="33">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="34">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="35">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:25" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" s="16" customFormat="1" ht="16.5" customHeight="1">
       <c r="A9" s="8" t="s">
         <v>1</v>
       </c>
@@ -1233,8 +1355,26 @@
       <c r="Y9" s="7">
         <v>1</v>
       </c>
+      <c r="Z9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="33">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="34">
+        <v>1</v>
+      </c>
+      <c r="AE9" s="35">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:25" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" s="16" customFormat="1" ht="16.5" customHeight="1">
       <c r="A10" s="8" t="s">
         <v>2</v>
       </c>
@@ -1310,8 +1450,26 @@
       <c r="Y10" s="7">
         <v>0</v>
       </c>
+      <c r="Z10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="33">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="34">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="35">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:25" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" s="16" customFormat="1" ht="16.5" customHeight="1">
       <c r="A11" s="9" t="s">
         <v>3</v>
       </c>
@@ -1387,8 +1545,26 @@
       <c r="Y11" s="7">
         <v>1</v>
       </c>
+      <c r="Z11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="33">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="34">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="35">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:25" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:31" s="16" customFormat="1" ht="16.5" customHeight="1">
       <c r="A12" s="9" t="s">
         <v>4</v>
       </c>
@@ -1464,8 +1640,26 @@
       <c r="Y12" s="7">
         <v>1</v>
       </c>
+      <c r="Z12" s="5">
+        <v>2</v>
+      </c>
+      <c r="AA12" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB12" s="7">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="33">
+        <v>1</v>
+      </c>
+      <c r="AD12" s="34">
+        <v>1</v>
+      </c>
+      <c r="AE12" s="35">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:25" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31" s="16" customFormat="1" ht="16.5" customHeight="1">
       <c r="A13" s="9" t="s">
         <v>5</v>
       </c>
@@ -1541,8 +1735,26 @@
       <c r="Y13" s="7">
         <v>0</v>
       </c>
+      <c r="Z13" s="5">
+        <v>2</v>
+      </c>
+      <c r="AA13" s="6">
+        <v>2</v>
+      </c>
+      <c r="AB13" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="33">
+        <v>3</v>
+      </c>
+      <c r="AD13" s="34">
+        <v>3</v>
+      </c>
+      <c r="AE13" s="35">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:25" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:31" s="16" customFormat="1" ht="16.5" customHeight="1">
       <c r="A14" s="9" t="s">
         <v>6</v>
       </c>
@@ -1618,8 +1830,26 @@
       <c r="Y14" s="7">
         <v>1</v>
       </c>
+      <c r="Z14" s="5">
+        <v>4</v>
+      </c>
+      <c r="AA14" s="6">
+        <v>2</v>
+      </c>
+      <c r="AB14" s="7">
+        <v>2</v>
+      </c>
+      <c r="AC14" s="33">
+        <v>2</v>
+      </c>
+      <c r="AD14" s="34">
+        <v>2</v>
+      </c>
+      <c r="AE14" s="35">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:25" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31" s="16" customFormat="1" ht="16.5" customHeight="1">
       <c r="A15" s="9" t="s">
         <v>7</v>
       </c>
@@ -1695,8 +1925,26 @@
       <c r="Y15" s="7">
         <v>3</v>
       </c>
+      <c r="Z15" s="5">
+        <v>6</v>
+      </c>
+      <c r="AA15" s="6">
+        <v>5</v>
+      </c>
+      <c r="AB15" s="7">
+        <v>1</v>
+      </c>
+      <c r="AC15" s="33">
+        <v>7</v>
+      </c>
+      <c r="AD15" s="34">
+        <v>4</v>
+      </c>
+      <c r="AE15" s="35">
+        <v>3</v>
+      </c>
     </row>
-    <row r="16" spans="1:25" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:31" s="16" customFormat="1" ht="16.5" customHeight="1">
       <c r="A16" s="9" t="s">
         <v>8</v>
       </c>
@@ -1772,8 +2020,26 @@
       <c r="Y16" s="7">
         <v>2</v>
       </c>
+      <c r="Z16" s="5">
+        <v>6</v>
+      </c>
+      <c r="AA16" s="6">
+        <v>6</v>
+      </c>
+      <c r="AB16" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="33">
+        <v>8</v>
+      </c>
+      <c r="AD16" s="34">
+        <v>8</v>
+      </c>
+      <c r="AE16" s="35">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:25" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:31" s="16" customFormat="1" ht="16.5" customHeight="1">
       <c r="A17" s="9" t="s">
         <v>9</v>
       </c>
@@ -1849,8 +2115,26 @@
       <c r="Y17" s="7">
         <v>5</v>
       </c>
+      <c r="Z17" s="5">
+        <v>12</v>
+      </c>
+      <c r="AA17" s="6">
+        <v>9</v>
+      </c>
+      <c r="AB17" s="7">
+        <v>3</v>
+      </c>
+      <c r="AC17" s="33">
+        <v>11</v>
+      </c>
+      <c r="AD17" s="34">
+        <v>8</v>
+      </c>
+      <c r="AE17" s="35">
+        <v>3</v>
+      </c>
     </row>
-    <row r="18" spans="1:25" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:31" s="16" customFormat="1" ht="16.5" customHeight="1">
       <c r="A18" s="9" t="s">
         <v>10</v>
       </c>
@@ -1926,8 +2210,26 @@
       <c r="Y18" s="7">
         <v>7</v>
       </c>
+      <c r="Z18" s="5">
+        <v>16</v>
+      </c>
+      <c r="AA18" s="6">
+        <v>11</v>
+      </c>
+      <c r="AB18" s="7">
+        <v>5</v>
+      </c>
+      <c r="AC18" s="33">
+        <v>15</v>
+      </c>
+      <c r="AD18" s="34">
+        <v>11</v>
+      </c>
+      <c r="AE18" s="35">
+        <v>4</v>
+      </c>
     </row>
-    <row r="19" spans="1:25" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:31" s="16" customFormat="1" ht="16.5" customHeight="1">
       <c r="A19" s="9" t="s">
         <v>11</v>
       </c>
@@ -2003,8 +2305,26 @@
       <c r="Y19" s="7">
         <v>7</v>
       </c>
+      <c r="Z19" s="5">
+        <v>30</v>
+      </c>
+      <c r="AA19" s="6">
+        <v>22</v>
+      </c>
+      <c r="AB19" s="7">
+        <v>8</v>
+      </c>
+      <c r="AC19" s="33">
+        <v>25</v>
+      </c>
+      <c r="AD19" s="34">
+        <v>20</v>
+      </c>
+      <c r="AE19" s="35">
+        <v>5</v>
+      </c>
     </row>
-    <row r="20" spans="1:25" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:31" s="16" customFormat="1" ht="16.5" customHeight="1">
       <c r="A20" s="9" t="s">
         <v>12</v>
       </c>
@@ -2080,8 +2400,26 @@
       <c r="Y20" s="7">
         <v>20</v>
       </c>
+      <c r="Z20" s="5">
+        <v>43</v>
+      </c>
+      <c r="AA20" s="6">
+        <v>31</v>
+      </c>
+      <c r="AB20" s="7">
+        <v>12</v>
+      </c>
+      <c r="AC20" s="33">
+        <v>33</v>
+      </c>
+      <c r="AD20" s="34">
+        <v>22</v>
+      </c>
+      <c r="AE20" s="35">
+        <v>11</v>
+      </c>
     </row>
-    <row r="21" spans="1:25" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:31" s="16" customFormat="1" ht="16.5" customHeight="1">
       <c r="A21" s="9" t="s">
         <v>13</v>
       </c>
@@ -2157,8 +2495,26 @@
       <c r="Y21" s="7">
         <v>26</v>
       </c>
+      <c r="Z21" s="5">
+        <v>45</v>
+      </c>
+      <c r="AA21" s="6">
+        <v>31</v>
+      </c>
+      <c r="AB21" s="7">
+        <v>14</v>
+      </c>
+      <c r="AC21" s="33">
+        <v>51</v>
+      </c>
+      <c r="AD21" s="34">
+        <v>36</v>
+      </c>
+      <c r="AE21" s="35">
+        <v>15</v>
+      </c>
     </row>
-    <row r="22" spans="1:25" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:31" s="16" customFormat="1" ht="16.5" customHeight="1">
       <c r="A22" s="9" t="s">
         <v>14</v>
       </c>
@@ -2234,8 +2590,26 @@
       <c r="Y22" s="7">
         <v>31</v>
       </c>
+      <c r="Z22" s="5">
+        <v>67</v>
+      </c>
+      <c r="AA22" s="6">
+        <v>37</v>
+      </c>
+      <c r="AB22" s="7">
+        <v>30</v>
+      </c>
+      <c r="AC22" s="33">
+        <v>72</v>
+      </c>
+      <c r="AD22" s="34">
+        <v>38</v>
+      </c>
+      <c r="AE22" s="35">
+        <v>34</v>
+      </c>
     </row>
-    <row r="23" spans="1:25" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:31" s="16" customFormat="1" ht="16.5" customHeight="1">
       <c r="A23" s="9" t="s">
         <v>15</v>
       </c>
@@ -2311,8 +2685,26 @@
       <c r="Y23" s="7">
         <v>40</v>
       </c>
+      <c r="Z23" s="5">
+        <v>45</v>
+      </c>
+      <c r="AA23" s="6">
+        <v>22</v>
+      </c>
+      <c r="AB23" s="7">
+        <v>23</v>
+      </c>
+      <c r="AC23" s="33">
+        <v>54</v>
+      </c>
+      <c r="AD23" s="34">
+        <v>23</v>
+      </c>
+      <c r="AE23" s="35">
+        <v>31</v>
+      </c>
     </row>
-    <row r="24" spans="1:25" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:31" s="16" customFormat="1" ht="16.5" customHeight="1">
       <c r="A24" s="9" t="s">
         <v>16</v>
       </c>
@@ -2388,8 +2780,26 @@
       <c r="Y24" s="7">
         <v>64</v>
       </c>
+      <c r="Z24" s="5">
+        <v>120</v>
+      </c>
+      <c r="AA24" s="6">
+        <v>51</v>
+      </c>
+      <c r="AB24" s="7">
+        <v>69</v>
+      </c>
+      <c r="AC24" s="33">
+        <v>71</v>
+      </c>
+      <c r="AD24" s="34">
+        <v>34</v>
+      </c>
+      <c r="AE24" s="35">
+        <v>37</v>
+      </c>
     </row>
-    <row r="25" spans="1:25" s="16" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" s="16" customFormat="1" ht="13.5" thickBot="1">
       <c r="A25" s="10" t="s">
         <v>17</v>
       </c>
@@ -2465,9 +2875,29 @@
       <c r="Y25" s="13">
         <v>71</v>
       </c>
+      <c r="Z25" s="11">
+        <v>96</v>
+      </c>
+      <c r="AA25" s="12">
+        <v>47</v>
+      </c>
+      <c r="AB25" s="13">
+        <v>49</v>
+      </c>
+      <c r="AC25" s="36">
+        <v>96</v>
+      </c>
+      <c r="AD25" s="37">
+        <v>38</v>
+      </c>
+      <c r="AE25" s="38">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
+    <mergeCell ref="AC4:AE4"/>
+    <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="Q4:S4"/>
     <mergeCell ref="T4:V4"/>
     <mergeCell ref="W4:Y4"/>

</xml_diff>